<commit_message>
Edit data so M_obs is total smolts
</commit_message>
<xml_diff>
--- a/data/Coho NPRB IPM column descriptions.xlsx
+++ b/data/Coho NPRB IPM column descriptions.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\nmfs.local\AKC-ABL\Users\Scott.Vulstek\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Buhle\My Application Data\R\AukeCoho\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>calendar_year</t>
   </si>
@@ -138,25 +138,25 @@
   </si>
   <si>
     <t>Estimated number of sport caught Auke Creek coho</t>
+  </si>
+  <si>
+    <t>total_smolt</t>
+  </si>
+  <si>
+    <t>The total number of smolt counted at the juvenile weir at Auke Creek</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color indexed="8"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -461,19 +461,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="94.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="94.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>18</v>
       </c>
@@ -481,7 +481,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -489,139 +489,147 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>3</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>4</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>5</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>6</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>7</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B10" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>8</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>9</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B12" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>10</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B13" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>15</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B14" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>16</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B15" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>17</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B16" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>11</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B17" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>12</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B18" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>13</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B19" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
         <v>14</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B20" t="s">
         <v>37</v>
       </c>
     </row>

</xml_diff>